<commit_message>
add honey's body health
</commit_message>
<xml_diff>
--- a/img/bodyhealth/妹妹的小日子.xlsx
+++ b/img/bodyhealth/妹妹的小日子.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FPGA_IP_GIT\python_learning\[4]bodyhealth\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\【2】github\kevinzhang0216.github.io\img\bodyhealth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77FF26F-7E6C-4E84-A99B-AE5809FB7B92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A00D630-ED3C-47F7-BBD3-FC4782FDAA5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{A1BF4A23-C03A-4241-8958-28E8C10D2F81}"/>
+    <workbookView xWindow="6580" yWindow="1800" windowWidth="19200" windowHeight="10060" xr2:uid="{A1BF4A23-C03A-4241-8958-28E8C10D2F81}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -196,6 +196,14 @@
   </si>
   <si>
     <t>2020.1.12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020.4.4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020.3.6</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -602,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{739F3719-822E-4DB3-AB1A-C17AD2F6E325}">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -824,6 +832,16 @@
         <v>41</v>
       </c>
     </row>
+    <row r="42" spans="1:1" ht="16.5">
+      <c r="A42" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="16.5">
+      <c r="A43" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
【发布】add my wife data
</commit_message>
<xml_diff>
--- a/img/bodyhealth/妹妹的小日子.xlsx
+++ b/img/bodyhealth/妹妹的小日子.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\【2】github\kevinzhang0216.github.io\img\bodyhealth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A00D630-ED3C-47F7-BBD3-FC4782FDAA5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142C53CE-45CF-444F-859C-1F97AE82B130}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6580" yWindow="1800" windowWidth="19200" windowHeight="10060" xr2:uid="{A1BF4A23-C03A-4241-8958-28E8C10D2F81}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="19200" windowHeight="10060" xr2:uid="{A1BF4A23-C03A-4241-8958-28E8C10D2F81}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -204,6 +204,14 @@
   </si>
   <si>
     <t>2020.3.6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020.5.4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020.6.1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -610,7 +618,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{739F3719-822E-4DB3-AB1A-C17AD2F6E325}">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
       <selection activeCell="A45" sqref="A45"/>
@@ -842,6 +850,16 @@
         <v>43</v>
       </c>
     </row>
+    <row r="44" spans="1:1" ht="16.5">
+      <c r="A44" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" ht="16.5">
+      <c r="A45" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>